<commit_message>
agregue hasta renta cuota 2
</commit_message>
<xml_diff>
--- a/Dataframes/cronotax.xlsx
+++ b/Dataframes/cronotax.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aieau\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\edinsonpb\cronotax\Dataframes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466552E1-F0E9-4EFB-848A-851FA0E5DD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD61E112-8E28-4125-990B-7F3974A860D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{36FFA0C7-75D1-44D7-BB55-D2E7574BCED4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="19" activeTab="21" xr2:uid="{36FFA0C7-75D1-44D7-BB55-D2E7574BCED4}"/>
   </bookViews>
   <sheets>
     <sheet name="declarantes" sheetId="1" r:id="rId1"/>
@@ -34,28 +34,29 @@
     <sheet name="reteicasantarosa" sheetId="31" r:id="rId19"/>
     <sheet name="icamedellin" sheetId="29" r:id="rId20"/>
     <sheet name="reteicamedellin" sheetId="30" r:id="rId21"/>
-    <sheet name="icabogotac" sheetId="28" r:id="rId22"/>
-    <sheet name="icabogotaa" sheetId="40" r:id="rId23"/>
-    <sheet name="reteicabogota" sheetId="27" r:id="rId24"/>
-    <sheet name="reteicatulua" sheetId="11" r:id="rId25"/>
-    <sheet name="icatulua" sheetId="21" r:id="rId26"/>
-    <sheet name="icapereira" sheetId="23" r:id="rId27"/>
-    <sheet name="reteicapereira" sheetId="24" r:id="rId28"/>
-    <sheet name="icadosquebradas" sheetId="25" r:id="rId29"/>
-    <sheet name="reteicadosquebradas" sheetId="26" r:id="rId30"/>
-    <sheet name="vehiculosBOGOTA" sheetId="18" r:id="rId31"/>
-    <sheet name="exogenaDIANgc" sheetId="13" r:id="rId32"/>
-    <sheet name="exogenaBOGOTA" sheetId="16" r:id="rId33"/>
-    <sheet name="exogenaPEREIRA" sheetId="17" r:id="rId34"/>
-    <sheet name="exogenaDOSQUEBRADAS" sheetId="20" r:id="rId35"/>
-    <sheet name="exogenaTULUA" sheetId="19" r:id="rId36"/>
-    <sheet name="exogenaDIANngc" sheetId="14" r:id="rId37"/>
+    <sheet name="icaarmenia" sheetId="42" r:id="rId22"/>
+    <sheet name="icabogotac" sheetId="28" r:id="rId23"/>
+    <sheet name="icabogotaa" sheetId="40" r:id="rId24"/>
+    <sheet name="reteicabogota" sheetId="27" r:id="rId25"/>
+    <sheet name="reteicatulua" sheetId="11" r:id="rId26"/>
+    <sheet name="icatulua" sheetId="21" r:id="rId27"/>
+    <sheet name="icapereira" sheetId="23" r:id="rId28"/>
+    <sheet name="reteicapereira" sheetId="24" r:id="rId29"/>
+    <sheet name="icadosquebradas" sheetId="25" r:id="rId30"/>
+    <sheet name="reteicadosquebradas" sheetId="26" r:id="rId31"/>
+    <sheet name="vehiculosBOGOTA" sheetId="18" r:id="rId32"/>
+    <sheet name="exogenaDIANgc" sheetId="13" r:id="rId33"/>
+    <sheet name="exogenaBOGOTA" sheetId="16" r:id="rId34"/>
+    <sheet name="exogenaPEREIRA" sheetId="17" r:id="rId35"/>
+    <sheet name="exogenaDOSQUEBRADAS" sheetId="20" r:id="rId36"/>
+    <sheet name="exogenaTULUA" sheetId="19" r:id="rId37"/>
+    <sheet name="exogenaDIANngc" sheetId="14" r:id="rId38"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId38"/>
+    <externalReference r:id="rId39"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">declarantes!$A$1:$R$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">declarantes!$A$1:$R$103</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dias!$A$1:$D$1097</definedName>
     <definedName name="estado" localSheetId="12">[1]resoluciones!$I$2:$I$65</definedName>
     <definedName name="estado">[1]resoluciones!$I$2:$I$64</definedName>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="648">
   <si>
     <t>Nit</t>
   </si>
@@ -2033,6 +2034,12 @@
   <si>
     <t>Naranjo Acevedo</t>
   </si>
+  <si>
+    <t>ARMENIA</t>
+  </si>
+  <si>
+    <t>ICAArmenia2024</t>
+  </si>
 </sst>
 </file>
 
@@ -2160,7 +2167,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2202,8 +2209,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares [0]" xfId="2" builtinId="6"/>
@@ -3099,10 +3104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4193D8-A317-4A4F-90EE-FC6E3DF425A1}">
-  <dimension ref="A1:T115"/>
+  <dimension ref="A1:T116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="J116" sqref="J116"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4088,19 +4093,19 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>900979503</v>
+        <v>900820009</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>25</v>
+        <v>315</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="4" t="s">
-        <v>173</v>
-      </c>
+      <c r="E26" s="4"/>
       <c r="F26" s="14"/>
       <c r="G26" s="11"/>
-      <c r="H26" s="12"/>
+      <c r="H26" s="12" t="s">
+        <v>646</v>
+      </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -4114,10 +4119,10 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>900274345</v>
+        <v>900979503</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -4140,10 +4145,10 @@
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>901602878</v>
+        <v>900274345</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>306</v>
+        <v>26</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -4166,48 +4171,29 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>901771767</v>
+        <v>901602878</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>590</v>
+        <v>306</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="F29" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>591</v>
-      </c>
+      <c r="F29" s="14"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="12"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
       <c r="M29" s="13"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="4" t="s">
-        <v>177</v>
-      </c>
+      <c r="O29" s="4"/>
       <c r="P29" s="4"/>
-      <c r="Q29" s="13" t="s">
-        <v>175</v>
-      </c>
+      <c r="Q29" s="13"/>
       <c r="R29" s="13"/>
-      <c r="T29" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -4221,22 +4207,34 @@
       <c r="E30" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="11"/>
+      <c r="F30" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>175</v>
+      </c>
       <c r="H30" s="12" t="s">
-        <v>277</v>
+        <v>591</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="M30" s="13"/>
       <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q30" s="13"/>
+      <c r="O30" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="13" t="s">
+        <v>175</v>
+      </c>
       <c r="R30" s="13"/>
       <c r="T30" t="s">
         <v>177</v>
@@ -4244,21 +4242,21 @@
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>18596354</v>
+        <v>901771767</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>28</v>
-      </c>
+        <v>590</v>
+      </c>
+      <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F31" s="10"/>
+        <v>173</v>
+      </c>
+      <c r="F31" s="14"/>
       <c r="G31" s="11"/>
-      <c r="H31" s="12"/>
+      <c r="H31" s="12" t="s">
+        <v>277</v>
+      </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -4266,75 +4264,67 @@
       <c r="M31" s="13"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
+      <c r="P31" s="4" t="s">
+        <v>277</v>
+      </c>
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
+      <c r="T31" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>42003950</v>
+        <v>18596354</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>178</v>
-      </c>
+      <c r="F32" s="10"/>
       <c r="G32" s="11"/>
-      <c r="H32" s="12" t="s">
-        <v>279</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="H32" s="12"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="13"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="P32" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q32" s="13" t="s">
-        <v>175</v>
-      </c>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
-      <c r="T32" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>94390997</v>
+        <v>42003950</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F33" s="10"/>
+      <c r="F33" s="10" t="s">
+        <v>178</v>
+      </c>
       <c r="G33" s="11"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="4"/>
+      <c r="H33" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="J33" s="4" t="s">
         <v>175</v>
       </c>
@@ -4344,85 +4334,98 @@
       <c r="L33" s="4"/>
       <c r="M33" s="13"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="13"/>
+      <c r="O33" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q33" s="13" t="s">
+        <v>175</v>
+      </c>
       <c r="R33" s="13"/>
+      <c r="T33" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>10119469</v>
+        <v>94390997</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F34" s="14" t="s">
-        <v>178</v>
-      </c>
+      <c r="F34" s="10"/>
       <c r="G34" s="11"/>
       <c r="H34" s="12"/>
       <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+      <c r="J34" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="K34" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="13"/>
       <c r="N34" s="4"/>
-      <c r="O34" s="4" t="s">
-        <v>177</v>
-      </c>
+      <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
-      <c r="S34" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>1088330427</v>
+        <v>10119469</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F35" s="14"/>
+      <c r="F35" s="14" t="s">
+        <v>178</v>
+      </c>
       <c r="G35" s="11"/>
       <c r="H35" s="12"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
+      <c r="K35" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="L35" s="4"/>
       <c r="M35" s="13"/>
       <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
+      <c r="O35" s="4" t="s">
+        <v>177</v>
+      </c>
       <c r="P35" s="4"/>
       <c r="Q35" s="13"/>
       <c r="R35" s="13"/>
+      <c r="S35" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>52368446</v>
+        <v>1088330427</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
@@ -4433,9 +4436,7 @@
       <c r="H36" s="12"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
-      <c r="K36" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="13"/>
       <c r="N36" s="4"/>
@@ -4446,13 +4447,13 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>8355265</v>
+        <v>52368446</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
@@ -4476,13 +4477,13 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>4538104</v>
+        <v>8355265</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
@@ -4493,7 +4494,9 @@
       <c r="H38" s="12"/>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
+      <c r="K38" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="L38" s="4"/>
       <c r="M38" s="13"/>
       <c r="N38" s="4"/>
@@ -4504,13 +4507,13 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>22590438</v>
+        <v>4538104</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
@@ -4521,9 +4524,7 @@
       <c r="H39" s="12"/>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
-      <c r="K39" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="13"/>
       <c r="N39" s="4"/>
@@ -4534,29 +4535,23 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>32711990</v>
+        <v>22590438</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F40" s="14" t="s">
-        <v>178</v>
-      </c>
+      <c r="F40" s="14"/>
       <c r="G40" s="11"/>
-      <c r="H40" s="12" t="s">
-        <v>277</v>
-      </c>
+      <c r="H40" s="12"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="J40" s="4"/>
       <c r="K40" s="4" t="s">
         <v>175</v>
       </c>
@@ -4565,33 +4560,34 @@
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
       <c r="P40" s="4"/>
-      <c r="Q40" s="13" t="s">
-        <v>175</v>
-      </c>
+      <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
-      <c r="T40" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>42059199</v>
+        <v>32711990</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F41" s="14"/>
+      <c r="F41" s="14" t="s">
+        <v>178</v>
+      </c>
       <c r="G41" s="11"/>
-      <c r="H41" s="12"/>
+      <c r="H41" s="12" t="s">
+        <v>277</v>
+      </c>
       <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
+      <c r="J41" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="K41" s="4" t="s">
         <v>175</v>
       </c>
@@ -4600,18 +4596,23 @@
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="13"/>
+      <c r="Q41" s="13" t="s">
+        <v>175</v>
+      </c>
       <c r="R41" s="13"/>
+      <c r="T41" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>42160142</v>
+        <v>42059199</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
@@ -4635,13 +4636,13 @@
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>24934404</v>
+        <v>42160142</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
@@ -4652,7 +4653,9 @@
       <c r="H43" s="12"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
+      <c r="K43" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="L43" s="4"/>
       <c r="M43" s="13"/>
       <c r="N43" s="4"/>
@@ -4663,10 +4666,10 @@
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>24941913</v>
+        <v>24934404</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>52</v>
@@ -4680,9 +4683,7 @@
       <c r="H44" s="12"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
-      <c r="K44" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="13"/>
       <c r="N44" s="4"/>
@@ -4690,33 +4691,26 @@
       <c r="P44" s="4"/>
       <c r="Q44" s="13"/>
       <c r="R44" s="13"/>
-      <c r="S44" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>10113836</v>
+        <v>24941913</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F45" s="14" t="s">
-        <v>178</v>
-      </c>
+      <c r="F45" s="14"/>
       <c r="G45" s="11"/>
       <c r="H45" s="12"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="J45" s="4"/>
       <c r="K45" s="4" t="s">
         <v>175</v>
       </c>
@@ -4727,26 +4721,33 @@
       <c r="P45" s="4"/>
       <c r="Q45" s="13"/>
       <c r="R45" s="13"/>
+      <c r="S45" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>1037580400</v>
+        <v>10113836</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F46" s="14"/>
+      <c r="F46" s="14" t="s">
+        <v>178</v>
+      </c>
       <c r="G46" s="11"/>
       <c r="H46" s="12"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
+      <c r="J46" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="K46" s="4" t="s">
         <v>175</v>
       </c>
@@ -4760,13 +4761,13 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>29134364</v>
+        <v>1037580400</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
@@ -4790,13 +4791,13 @@
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>29137079</v>
+        <v>29134364</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4" t="s">
@@ -4817,19 +4818,16 @@
       <c r="P48" s="4"/>
       <c r="Q48" s="13"/>
       <c r="R48" s="13"/>
-      <c r="S48" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>10000418</v>
+        <v>29137079</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4" t="s">
@@ -4856,13 +4854,13 @@
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>9776933</v>
+        <v>10000418</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4" t="s">
@@ -4889,13 +4887,13 @@
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>15525656</v>
+        <v>9776933</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4" t="s">
@@ -4916,16 +4914,19 @@
       <c r="P51" s="4"/>
       <c r="Q51" s="13"/>
       <c r="R51" s="13"/>
+      <c r="S51" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>1088274337</v>
+        <v>15525656</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>308</v>
+        <v>65</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4" t="s">
@@ -4949,13 +4950,13 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>14880679</v>
+        <v>1088274337</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>67</v>
+        <v>308</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
@@ -4979,13 +4980,13 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>18591946</v>
+        <v>14880679</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D54" s="4"/>
       <c r="E54" s="4" t="s">
@@ -5009,13 +5010,13 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>10125391</v>
+        <v>18591946</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
@@ -5026,7 +5027,9 @@
       <c r="H55" s="12"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
-      <c r="K55" s="4"/>
+      <c r="K55" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="L55" s="4"/>
       <c r="M55" s="13"/>
       <c r="N55" s="4"/>
@@ -5037,88 +5040,86 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>18613669</v>
+        <v>10125391</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F56" s="14" t="s">
-        <v>178</v>
-      </c>
+      <c r="F56" s="14"/>
       <c r="G56" s="11"/>
-      <c r="H56" s="12" t="s">
-        <v>277</v>
-      </c>
+      <c r="H56" s="12"/>
       <c r="I56" s="4"/>
-      <c r="J56" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="K56" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
       <c r="L56" s="4"/>
       <c r="M56" s="13"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="P56" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q56" s="13" t="s">
-        <v>175</v>
-      </c>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="13"/>
       <c r="R56" s="13"/>
-      <c r="T56" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>42124850</v>
+        <v>18613669</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>307</v>
+        <v>73</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F57" s="14"/>
+      <c r="F57" s="14" t="s">
+        <v>178</v>
+      </c>
       <c r="G57" s="11"/>
-      <c r="H57" s="12"/>
+      <c r="H57" s="12" t="s">
+        <v>277</v>
+      </c>
       <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
+      <c r="J57" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="K57" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L57" s="4"/>
       <c r="M57" s="13"/>
       <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
-      <c r="P57" s="4"/>
-      <c r="Q57" s="13"/>
+      <c r="O57" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="P57" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q57" s="13" t="s">
+        <v>175</v>
+      </c>
       <c r="R57" s="13"/>
+      <c r="T57" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>10138765</v>
+        <v>42124850</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>75</v>
+        <v>307</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
@@ -5126,43 +5127,29 @@
       </c>
       <c r="F58" s="14"/>
       <c r="G58" s="11"/>
-      <c r="H58" s="12" t="s">
-        <v>277</v>
-      </c>
+      <c r="H58" s="12"/>
       <c r="I58" s="4"/>
-      <c r="J58" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="J58" s="4"/>
       <c r="K58" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L58" s="4"/>
       <c r="M58" s="13"/>
       <c r="N58" s="4"/>
-      <c r="O58" s="4" t="s">
-        <v>177</v>
-      </c>
+      <c r="O58" s="4"/>
       <c r="P58" s="4"/>
-      <c r="Q58" s="13" t="s">
-        <v>175</v>
-      </c>
+      <c r="Q58" s="13"/>
       <c r="R58" s="13"/>
-      <c r="S58" t="s">
-        <v>175</v>
-      </c>
-      <c r="T58" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>24761147</v>
+        <v>10138765</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
@@ -5170,29 +5157,43 @@
       </c>
       <c r="F59" s="14"/>
       <c r="G59" s="11"/>
-      <c r="H59" s="12"/>
+      <c r="H59" s="12" t="s">
+        <v>277</v>
+      </c>
       <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
+      <c r="J59" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="K59" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L59" s="4"/>
       <c r="M59" s="13"/>
       <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
+      <c r="O59" s="4" t="s">
+        <v>177</v>
+      </c>
       <c r="P59" s="4"/>
-      <c r="Q59" s="13"/>
+      <c r="Q59" s="13" t="s">
+        <v>175</v>
+      </c>
       <c r="R59" s="13"/>
+      <c r="S59" t="s">
+        <v>175</v>
+      </c>
+      <c r="T59" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>24925995</v>
+        <v>24761147</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
@@ -5216,13 +5217,13 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>23619081</v>
+        <v>24925995</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
@@ -5246,10 +5247,10 @@
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>23618109</v>
+        <v>23619081</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>70</v>
@@ -5276,13 +5277,13 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>42151996</v>
+        <v>23618109</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
@@ -5306,13 +5307,13 @@
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>41908742</v>
+        <v>42151996</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
@@ -5336,87 +5337,87 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>10133430</v>
+        <v>41908742</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F65" s="14" t="s">
-        <v>178</v>
-      </c>
+      <c r="F65" s="14"/>
       <c r="G65" s="11"/>
-      <c r="H65" s="12" t="s">
-        <v>277</v>
-      </c>
+      <c r="H65" s="12"/>
       <c r="I65" s="4"/>
-      <c r="J65" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="J65" s="4"/>
       <c r="K65" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L65" s="4"/>
       <c r="M65" s="13"/>
       <c r="N65" s="4"/>
-      <c r="O65" s="4" t="s">
-        <v>177</v>
-      </c>
+      <c r="O65" s="4"/>
       <c r="P65" s="4"/>
       <c r="Q65" s="13"/>
       <c r="R65" s="13"/>
-      <c r="S65" t="s">
-        <v>175</v>
-      </c>
-      <c r="T65" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>10029541</v>
+        <v>10133430</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F66" s="14"/>
+      <c r="F66" s="14" t="s">
+        <v>178</v>
+      </c>
       <c r="G66" s="11"/>
-      <c r="H66" s="12"/>
+      <c r="H66" s="12" t="s">
+        <v>277</v>
+      </c>
       <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
+      <c r="J66" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="K66" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L66" s="4"/>
       <c r="M66" s="13"/>
       <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
+      <c r="O66" s="4" t="s">
+        <v>177</v>
+      </c>
       <c r="P66" s="4"/>
       <c r="Q66" s="13"/>
       <c r="R66" s="13"/>
+      <c r="S66" t="s">
+        <v>175</v>
+      </c>
+      <c r="T66" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <v>1088014975</v>
+        <v>10029541</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
@@ -5440,13 +5441,13 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>29275129</v>
+        <v>1088014975</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
@@ -5470,13 +5471,13 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>94479341</v>
+        <v>29275129</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
@@ -5500,13 +5501,13 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>70190961</v>
+        <v>94479341</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
@@ -5530,13 +5531,13 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <v>52546115</v>
+        <v>70190961</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4" t="s">
@@ -5560,13 +5561,13 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <v>10025319</v>
+        <v>52546115</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
@@ -5590,13 +5591,13 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <v>10244919</v>
+        <v>10025319</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
@@ -5607,7 +5608,9 @@
       <c r="H73" s="12"/>
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
+      <c r="K73" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="L73" s="4"/>
       <c r="M73" s="13"/>
       <c r="N73" s="4"/>
@@ -5618,13 +5621,13 @@
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>7539221</v>
+        <v>10244919</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
@@ -5646,13 +5649,13 @@
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>4577556</v>
+        <v>7539221</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
@@ -5663,9 +5666,7 @@
       <c r="H75" s="12"/>
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
-      <c r="K75" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="K75" s="4"/>
       <c r="L75" s="4"/>
       <c r="M75" s="13"/>
       <c r="N75" s="4"/>
@@ -5676,13 +5677,13 @@
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>20039738</v>
+        <v>4577556</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4" t="s">
@@ -5706,13 +5707,13 @@
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>79338411</v>
+        <v>20039738</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4" t="s">
@@ -5736,13 +5737,13 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>6241137</v>
+        <v>79338411</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
@@ -5766,13 +5767,13 @@
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <v>42024973</v>
+        <v>6241137</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
@@ -5782,9 +5783,7 @@
       <c r="G79" s="11"/>
       <c r="H79" s="12"/>
       <c r="I79" s="4"/>
-      <c r="J79" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="J79" s="4"/>
       <c r="K79" s="4" t="s">
         <v>175</v>
       </c>
@@ -5798,13 +5797,13 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>1088291110</v>
+        <v>42024973</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4" t="s">
@@ -5814,7 +5813,9 @@
       <c r="G80" s="11"/>
       <c r="H80" s="12"/>
       <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
+      <c r="J80" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="K80" s="4" t="s">
         <v>175</v>
       </c>
@@ -5828,13 +5829,13 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>18613617</v>
+        <v>1088291110</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4" t="s">
@@ -5858,13 +5859,13 @@
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>10062862</v>
+        <v>18613617</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4" t="s">
@@ -5888,89 +5889,89 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <v>42058708</v>
+        <v>10062862</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F83" s="14" t="s">
-        <v>174</v>
-      </c>
+      <c r="F83" s="14"/>
       <c r="G83" s="11"/>
-      <c r="H83" s="12" t="s">
-        <v>277</v>
-      </c>
+      <c r="H83" s="12"/>
       <c r="I83" s="4"/>
-      <c r="J83" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="J83" s="4"/>
       <c r="K83" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L83" s="4"/>
       <c r="M83" s="13"/>
       <c r="N83" s="4"/>
-      <c r="O83" s="4" t="s">
-        <v>177</v>
-      </c>
+      <c r="O83" s="4"/>
       <c r="P83" s="4"/>
-      <c r="Q83" s="13" t="s">
-        <v>175</v>
-      </c>
+      <c r="Q83" s="13"/>
       <c r="R83" s="13"/>
-      <c r="S83" t="s">
-        <v>175</v>
-      </c>
-      <c r="T83" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
-        <v>1088347035</v>
+        <v>42058708</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>36</v>
+        <v>124</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F84" s="14"/>
+      <c r="F84" s="14" t="s">
+        <v>174</v>
+      </c>
       <c r="G84" s="11"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="4"/>
+      <c r="H84" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="K84" s="4" t="s">
         <v>175</v>
       </c>
       <c r="L84" s="4"/>
       <c r="M84" s="13"/>
-      <c r="N84" s="13"/>
-      <c r="O84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4" t="s">
+        <v>177</v>
+      </c>
       <c r="P84" s="4"/>
-      <c r="Q84" s="13"/>
+      <c r="Q84" s="13" t="s">
+        <v>175</v>
+      </c>
       <c r="R84" s="13"/>
+      <c r="S84" t="s">
+        <v>175</v>
+      </c>
+      <c r="T84" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
-        <v>1125783111</v>
+        <v>1088347035</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>127</v>
+        <v>36</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4" t="s">
@@ -5994,17 +5995,15 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
-        <v>1088276883</v>
+        <v>1125783111</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>175</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D86" s="4"/>
       <c r="E86" s="4" t="s">
         <v>180</v>
       </c>
@@ -6019,24 +6018,24 @@
       <c r="L86" s="4"/>
       <c r="M86" s="13"/>
       <c r="N86" s="13"/>
-      <c r="O86" s="4" t="s">
-        <v>177</v>
-      </c>
+      <c r="O86" s="4"/>
       <c r="P86" s="4"/>
       <c r="Q86" s="13"/>
       <c r="R86" s="13"/>
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
-        <v>1088256970</v>
+        <v>1088276883</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D87" s="4"/>
+        <v>129</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="E87" s="4" t="s">
         <v>180</v>
       </c>
@@ -6051,20 +6050,22 @@
       <c r="L87" s="4"/>
       <c r="M87" s="13"/>
       <c r="N87" s="13"/>
-      <c r="O87" s="4"/>
+      <c r="O87" s="4" t="s">
+        <v>177</v>
+      </c>
       <c r="P87" s="4"/>
       <c r="Q87" s="13"/>
       <c r="R87" s="13"/>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
-        <v>1118236429</v>
+        <v>1088256970</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
@@ -6088,13 +6089,13 @@
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
-        <v>1127250111</v>
+        <v>1118236429</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
@@ -6118,13 +6119,13 @@
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
-        <v>42113099</v>
+        <v>1127250111</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4" t="s">
@@ -6148,13 +6149,13 @@
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <v>6454014</v>
+        <v>42113099</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
@@ -6178,13 +6179,13 @@
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>24940525</v>
+        <v>6454014</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4" t="s">
@@ -6208,13 +6209,13 @@
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>4516590</v>
+        <v>24940525</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
@@ -6238,13 +6239,13 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>18616381</v>
+        <v>4516590</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
@@ -6255,7 +6256,9 @@
       <c r="H94" s="12"/>
       <c r="I94" s="12"/>
       <c r="J94" s="4"/>
-      <c r="K94" s="4"/>
+      <c r="K94" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="L94" s="4"/>
       <c r="M94" s="13"/>
       <c r="N94" s="13"/>
@@ -6266,13 +6269,13 @@
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <v>9871410</v>
+        <v>18616381</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
@@ -6294,13 +6297,13 @@
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <v>1088251266</v>
+        <v>9871410</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
@@ -6311,9 +6314,7 @@
       <c r="H96" s="12"/>
       <c r="I96" s="12"/>
       <c r="J96" s="4"/>
-      <c r="K96" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="K96" s="4"/>
       <c r="L96" s="4"/>
       <c r="M96" s="13"/>
       <c r="N96" s="13"/>
@@ -6324,13 +6325,13 @@
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <v>1088336898</v>
+        <v>1088251266</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
@@ -6354,13 +6355,13 @@
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>16362043</v>
+        <v>1088336898</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4" t="s">
@@ -6384,13 +6385,13 @@
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>10031761</v>
+        <v>16362043</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>87</v>
+        <v>151</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4" t="s">
@@ -6414,13 +6415,13 @@
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <v>66949650</v>
+        <v>10031761</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>154</v>
+        <v>87</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4" t="s">
@@ -6444,13 +6445,13 @@
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
-        <v>79128270</v>
+        <v>66949650</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4" t="s">
@@ -6473,42 +6474,44 @@
       <c r="R101" s="13"/>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A102" s="5">
-        <v>42067155</v>
-      </c>
-      <c r="B102" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D102" s="6"/>
-      <c r="E102" s="6" t="s">
+      <c r="A102" s="3">
+        <v>79128270</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="F102" s="15"/>
-      <c r="G102" s="16"/>
-      <c r="H102" s="17"/>
-      <c r="I102" s="6"/>
-      <c r="J102" s="6"/>
-      <c r="K102" s="4"/>
-      <c r="L102" s="6"/>
-      <c r="M102" s="18"/>
-      <c r="N102" s="6"/>
-      <c r="O102" s="6"/>
-      <c r="P102" s="6"/>
-      <c r="Q102" s="18"/>
-      <c r="R102" s="18"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="11"/>
+      <c r="H102" s="12"/>
+      <c r="I102" s="12"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="L102" s="4"/>
+      <c r="M102" s="13"/>
+      <c r="N102" s="13"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4"/>
+      <c r="Q102" s="13"/>
+      <c r="R102" s="13"/>
     </row>
     <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" s="5">
-        <v>52737692</v>
+        <v>42067155</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>577</v>
+        <v>158</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>578</v>
+        <v>159</v>
       </c>
       <c r="D103" s="6"/>
       <c r="E103" s="6" t="s">
@@ -6516,9 +6519,7 @@
       </c>
       <c r="F103" s="15"/>
       <c r="G103" s="16"/>
-      <c r="H103" s="17" t="s">
-        <v>276</v>
-      </c>
+      <c r="H103" s="17"/>
       <c r="I103" s="6"/>
       <c r="J103" s="6"/>
       <c r="K103" s="4"/>
@@ -6529,19 +6530,16 @@
       <c r="P103" s="6"/>
       <c r="Q103" s="18"/>
       <c r="R103" s="18"/>
-      <c r="T103" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
-        <v>25153867</v>
+        <v>52737692</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>309</v>
+        <v>577</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>310</v>
+        <v>578</v>
       </c>
       <c r="D104" s="6"/>
       <c r="E104" s="6" t="s">
@@ -6549,12 +6547,12 @@
       </c>
       <c r="F104" s="15"/>
       <c r="G104" s="16"/>
-      <c r="H104" s="17"/>
+      <c r="H104" s="17" t="s">
+        <v>276</v>
+      </c>
       <c r="I104" s="6"/>
       <c r="J104" s="6"/>
-      <c r="K104" s="4" t="s">
-        <v>175</v>
-      </c>
+      <c r="K104" s="4"/>
       <c r="L104" s="6"/>
       <c r="M104" s="18"/>
       <c r="N104" s="6"/>
@@ -6562,33 +6560,49 @@
       <c r="P104" s="6"/>
       <c r="Q104" s="18"/>
       <c r="R104" s="18"/>
+      <c r="T104" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A105" s="32">
-        <v>1125801521</v>
-      </c>
-      <c r="B105" s="23" t="s">
-        <v>592</v>
-      </c>
-      <c r="C105" s="23" t="s">
-        <v>593</v>
-      </c>
-      <c r="E105" s="23" t="s">
+      <c r="A105" s="5">
+        <v>25153867</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="K105" s="23" t="s">
+      <c r="F105" s="15"/>
+      <c r="G105" s="16"/>
+      <c r="H105" s="17"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="4" t="s">
         <v>175</v>
       </c>
+      <c r="L105" s="6"/>
+      <c r="M105" s="18"/>
+      <c r="N105" s="6"/>
+      <c r="O105" s="6"/>
+      <c r="P105" s="6"/>
+      <c r="Q105" s="18"/>
+      <c r="R105" s="18"/>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="32">
-        <v>18591578</v>
+        <v>1125801521</v>
       </c>
       <c r="B106" s="23" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E106" s="23" t="s">
         <v>180</v>
@@ -6599,13 +6613,13 @@
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="32">
-        <v>25156789</v>
+        <v>18591578</v>
       </c>
       <c r="B107" s="23" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C107" s="23" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E107" s="23" t="s">
         <v>180</v>
@@ -6616,13 +6630,13 @@
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" s="32">
-        <v>52341926</v>
+        <v>25156789</v>
       </c>
       <c r="B108" s="23" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C108" s="23" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E108" s="23" t="s">
         <v>180</v>
@@ -6633,13 +6647,13 @@
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="32">
-        <v>1031643471</v>
+        <v>52341926</v>
       </c>
       <c r="B109" s="23" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C109" s="23" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E109" s="23" t="s">
         <v>180</v>
@@ -6650,13 +6664,13 @@
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="32">
-        <v>79590573</v>
+        <v>1031643471</v>
       </c>
       <c r="B110" s="23" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C110" s="23" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E110" s="23" t="s">
         <v>180</v>
@@ -6667,13 +6681,13 @@
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="32">
-        <v>1087999135</v>
+        <v>79590573</v>
       </c>
       <c r="B111" s="23" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C111" s="23" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="E111" s="23" t="s">
         <v>180</v>
@@ -6684,13 +6698,13 @@
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="32">
-        <v>14970629</v>
+        <v>1087999135</v>
       </c>
       <c r="B112" s="23" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C112" s="23" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E112" s="23" t="s">
         <v>180</v>
@@ -6701,13 +6715,13 @@
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="32">
-        <v>10097783</v>
+        <v>14970629</v>
       </c>
       <c r="B113" s="23" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C113" s="23" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E113" s="23" t="s">
         <v>180</v>
@@ -6718,41 +6732,58 @@
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="32">
-        <v>1088288292</v>
+        <v>10097783</v>
       </c>
       <c r="B114" s="23" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C114" s="23" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E114" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="H114" t="s">
-        <v>277</v>
-      </c>
       <c r="K114" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="T114" t="s">
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A115" s="32">
+        <v>1088288292</v>
+      </c>
+      <c r="B115" s="23" t="s">
+        <v>610</v>
+      </c>
+      <c r="C115" s="23" t="s">
+        <v>611</v>
+      </c>
+      <c r="E115" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="H115" t="s">
+        <v>277</v>
+      </c>
+      <c r="K115" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="T115" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A115" s="33">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A116" s="32">
         <v>1088316247</v>
       </c>
-      <c r="B115" s="34" t="s">
+      <c r="B116" s="23" t="s">
         <v>644</v>
       </c>
-      <c r="C115" s="34" t="s">
+      <c r="C116" s="23" t="s">
         <v>645</v>
       </c>
-      <c r="E115" s="34" t="s">
+      <c r="E116" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="J115" t="s">
+      <c r="J116" t="s">
         <v>175</v>
       </c>
     </row>
@@ -13895,8 +13926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9742DF40-FC3F-4F3E-A4F3-058FDFFF2FBE}">
   <dimension ref="A1:AR129"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53849,10 +53880,10 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54320,6 +54351,116 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22978039-1543-4DF0-A3D8-F1CAD6292EF2}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25">
+        <v>45807</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25">
+        <v>45803</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25">
+        <v>45803</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25">
+        <v>45804</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25">
+        <v>45804</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="25">
+        <v>45805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="25">
+        <v>45805</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="25">
+        <v>45806</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="25">
+        <v>45806</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="25">
+        <v>45807</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B60C46-C0EC-47FA-A6FF-2752DA5B9277}">
   <dimension ref="A1:W11"/>
   <sheetViews>
@@ -55130,7 +55271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E797086-F05B-4A96-AB43-B898E4C9E9CA}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -55240,7 +55381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F58881-7BDA-49F7-962D-91B3476525F1}">
   <dimension ref="A1:S11"/>
   <sheetViews>
@@ -55910,7 +56051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33204E53-D2B8-45CC-AA3A-CE19C3715535}">
   <dimension ref="A1:M11"/>
   <sheetViews>
@@ -56385,7 +56526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D31948-19A8-4D23-ABCE-CE402CA20A53}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -56658,7 +56799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6D1D696-1D68-4E50-920F-7F99DA5CC643}">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -56832,12 +56973,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C96F31-27CE-48DA-9D66-B397132F1D6A}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57498,181 +57639,6 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B465BB48-ACD6-4F86-9031-0CEE9A3CDA80}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>570</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>612</v>
-      </c>
-      <c r="E1" s="25"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="25">
-        <v>45044</v>
-      </c>
-      <c r="C2" s="25">
-        <v>45408</v>
-      </c>
-      <c r="D2" s="25">
-        <v>45772</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="25">
-        <v>45044</v>
-      </c>
-      <c r="C3" s="25">
-        <v>45408</v>
-      </c>
-      <c r="D3" s="25">
-        <v>45772</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="25">
-        <v>45044</v>
-      </c>
-      <c r="C4" s="25">
-        <v>45408</v>
-      </c>
-      <c r="D4" s="25">
-        <v>45772</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="25">
-        <v>45044</v>
-      </c>
-      <c r="C5" s="25">
-        <v>45408</v>
-      </c>
-      <c r="D5" s="25">
-        <v>45772</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="25">
-        <v>45044</v>
-      </c>
-      <c r="C6" s="25">
-        <v>45408</v>
-      </c>
-      <c r="D6" s="25">
-        <v>45772</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" s="25">
-        <v>45044</v>
-      </c>
-      <c r="C7" s="25">
-        <v>45408</v>
-      </c>
-      <c r="D7" s="25">
-        <v>45772</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" s="25">
-        <v>45044</v>
-      </c>
-      <c r="C8" s="25">
-        <v>45408</v>
-      </c>
-      <c r="D8" s="25">
-        <v>45772</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="25">
-        <v>45044</v>
-      </c>
-      <c r="C9" s="25">
-        <v>45408</v>
-      </c>
-      <c r="D9" s="25">
-        <v>45772</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" s="25">
-        <v>45044</v>
-      </c>
-      <c r="C10" s="25">
-        <v>45408</v>
-      </c>
-      <c r="D10" s="25">
-        <v>45772</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" s="25">
-        <v>45044</v>
-      </c>
-      <c r="C11" s="25">
-        <v>45408</v>
-      </c>
-      <c r="D11" s="25">
-        <v>45772</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -58787,6 +58753,181 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B465BB48-ACD6-4F86-9031-0CEE9A3CDA80}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>570</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>612</v>
+      </c>
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="25">
+        <v>45044</v>
+      </c>
+      <c r="C2" s="25">
+        <v>45408</v>
+      </c>
+      <c r="D2" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25">
+        <v>45044</v>
+      </c>
+      <c r="C3" s="25">
+        <v>45408</v>
+      </c>
+      <c r="D3" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25">
+        <v>45044</v>
+      </c>
+      <c r="C4" s="25">
+        <v>45408</v>
+      </c>
+      <c r="D4" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25">
+        <v>45044</v>
+      </c>
+      <c r="C5" s="25">
+        <v>45408</v>
+      </c>
+      <c r="D5" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25">
+        <v>45044</v>
+      </c>
+      <c r="C6" s="25">
+        <v>45408</v>
+      </c>
+      <c r="D6" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="25">
+        <v>45044</v>
+      </c>
+      <c r="C7" s="25">
+        <v>45408</v>
+      </c>
+      <c r="D7" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="25">
+        <v>45044</v>
+      </c>
+      <c r="C8" s="25">
+        <v>45408</v>
+      </c>
+      <c r="D8" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="25">
+        <v>45044</v>
+      </c>
+      <c r="C9" s="25">
+        <v>45408</v>
+      </c>
+      <c r="D9" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="25">
+        <v>45044</v>
+      </c>
+      <c r="C10" s="25">
+        <v>45408</v>
+      </c>
+      <c r="D10" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" s="25">
+        <v>45044</v>
+      </c>
+      <c r="C11" s="25">
+        <v>45408</v>
+      </c>
+      <c r="D11" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CEC142-A635-4FB4-AA57-65CA601519CD}">
   <dimension ref="A1:S11"/>
   <sheetViews>
@@ -59457,7 +59598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809C0209-8328-4D0B-987B-19C4CF057C79}">
   <dimension ref="B2"/>
   <sheetViews>
@@ -59477,7 +59618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBAF3D5-3C70-4001-9C40-B0AE15F873AA}">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -59651,7 +59792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{253B0B9A-1D50-46F0-B1D1-FE11EE9F60DF}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -59791,7 +59932,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B316574-18F6-4D00-8401-078BA6DD5912}">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -59965,7 +60106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7C63A8-7A14-4B1C-8B0F-48E1F69FA19D}">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -60140,7 +60281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0664ACD4-377B-4BEA-B4B2-678D03599694}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -60280,7 +60421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A3B4FC-3E84-42CB-B04A-449200BBF9BD}">
   <dimension ref="A1:E101"/>
   <sheetViews>

</xml_diff>

<commit_message>
completando parcialmente el calendario
</commit_message>
<xml_diff>
--- a/Dataframes/cronotax.xlsx
+++ b/Dataframes/cronotax.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\edinsonpb\cronotax\Dataframes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD61E112-8E28-4125-990B-7F3974A860D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36015D1F-F714-4226-81AB-C791E85C8355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" firstSheet="19" activeTab="21" xr2:uid="{36FFA0C7-75D1-44D7-BB55-D2E7574BCED4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{36FFA0C7-75D1-44D7-BB55-D2E7574BCED4}"/>
   </bookViews>
   <sheets>
     <sheet name="declarantes" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="649">
   <si>
     <t>Nit</t>
   </si>
@@ -1010,9 +1010,6 @@
   </si>
   <si>
     <t>IMPCObim5-23</t>
-  </si>
-  <si>
-    <t>SUPERSOC22</t>
   </si>
   <si>
     <t>GLOBAL FINANCIAL CONSULTING GROUP S.A.S.</t>
@@ -2039,6 +2036,12 @@
   </si>
   <si>
     <t>ICAArmenia2024</t>
+  </si>
+  <si>
+    <t>SUPERSOC23</t>
+  </si>
+  <si>
+    <t>SUPERSOC24</t>
   </si>
 </sst>
 </file>
@@ -3106,8 +3109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4193D8-A317-4A4F-90EE-FC6E3DF425A1}">
   <dimension ref="A1:T116"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3187,10 +3190,10 @@
         <v>172</v>
       </c>
       <c r="S1" s="29" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="T1" s="29" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -4045,7 +4048,7 @@
         <v>900820009</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -4072,9 +4075,7 @@
         <v>175</v>
       </c>
       <c r="M25" s="13"/>
-      <c r="N25" s="4" t="s">
-        <v>176</v>
-      </c>
+      <c r="N25" s="4"/>
       <c r="O25" s="4" t="s">
         <v>177</v>
       </c>
@@ -4096,7 +4097,7 @@
         <v>900820009</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -4104,7 +4105,7 @@
       <c r="F26" s="14"/>
       <c r="G26" s="11"/>
       <c r="H26" s="12" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -4116,6 +4117,9 @@
       <c r="P26" s="4"/>
       <c r="Q26" s="13"/>
       <c r="R26" s="13"/>
+      <c r="T26" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -4174,7 +4178,7 @@
         <v>901602878</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -4200,7 +4204,7 @@
         <v>901771767</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -4214,7 +4218,7 @@
         <v>175</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
@@ -4245,7 +4249,7 @@
         <v>901771767</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -4953,7 +4957,7 @@
         <v>1088274337</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>50</v>
@@ -5116,7 +5120,7 @@
         <v>42124850</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>127</v>
@@ -6536,10 +6540,10 @@
         <v>52737692</v>
       </c>
       <c r="B104" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="C104" s="6" t="s">
         <v>577</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>578</v>
       </c>
       <c r="D104" s="6"/>
       <c r="E104" s="6" t="s">
@@ -6569,10 +6573,10 @@
         <v>25153867</v>
       </c>
       <c r="B105" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C105" s="6" t="s">
         <v>309</v>
-      </c>
-      <c r="C105" s="6" t="s">
-        <v>310</v>
       </c>
       <c r="D105" s="6"/>
       <c r="E105" s="6" t="s">
@@ -6599,10 +6603,10 @@
         <v>1125801521</v>
       </c>
       <c r="B106" s="23" t="s">
+        <v>591</v>
+      </c>
+      <c r="C106" s="23" t="s">
         <v>592</v>
-      </c>
-      <c r="C106" s="23" t="s">
-        <v>593</v>
       </c>
       <c r="E106" s="23" t="s">
         <v>180</v>
@@ -6616,10 +6620,10 @@
         <v>18591578</v>
       </c>
       <c r="B107" s="23" t="s">
+        <v>593</v>
+      </c>
+      <c r="C107" s="23" t="s">
         <v>594</v>
-      </c>
-      <c r="C107" s="23" t="s">
-        <v>595</v>
       </c>
       <c r="E107" s="23" t="s">
         <v>180</v>
@@ -6633,10 +6637,10 @@
         <v>25156789</v>
       </c>
       <c r="B108" s="23" t="s">
+        <v>595</v>
+      </c>
+      <c r="C108" s="23" t="s">
         <v>596</v>
-      </c>
-      <c r="C108" s="23" t="s">
-        <v>597</v>
       </c>
       <c r="E108" s="23" t="s">
         <v>180</v>
@@ -6650,10 +6654,10 @@
         <v>52341926</v>
       </c>
       <c r="B109" s="23" t="s">
+        <v>597</v>
+      </c>
+      <c r="C109" s="23" t="s">
         <v>598</v>
-      </c>
-      <c r="C109" s="23" t="s">
-        <v>599</v>
       </c>
       <c r="E109" s="23" t="s">
         <v>180</v>
@@ -6667,10 +6671,10 @@
         <v>1031643471</v>
       </c>
       <c r="B110" s="23" t="s">
+        <v>599</v>
+      </c>
+      <c r="C110" s="23" t="s">
         <v>600</v>
-      </c>
-      <c r="C110" s="23" t="s">
-        <v>601</v>
       </c>
       <c r="E110" s="23" t="s">
         <v>180</v>
@@ -6684,10 +6688,10 @@
         <v>79590573</v>
       </c>
       <c r="B111" s="23" t="s">
+        <v>601</v>
+      </c>
+      <c r="C111" s="23" t="s">
         <v>602</v>
-      </c>
-      <c r="C111" s="23" t="s">
-        <v>603</v>
       </c>
       <c r="E111" s="23" t="s">
         <v>180</v>
@@ -6701,10 +6705,10 @@
         <v>1087999135</v>
       </c>
       <c r="B112" s="23" t="s">
+        <v>603</v>
+      </c>
+      <c r="C112" s="23" t="s">
         <v>604</v>
-      </c>
-      <c r="C112" s="23" t="s">
-        <v>605</v>
       </c>
       <c r="E112" s="23" t="s">
         <v>180</v>
@@ -6718,10 +6722,10 @@
         <v>14970629</v>
       </c>
       <c r="B113" s="23" t="s">
+        <v>605</v>
+      </c>
+      <c r="C113" s="23" t="s">
         <v>606</v>
-      </c>
-      <c r="C113" s="23" t="s">
-        <v>607</v>
       </c>
       <c r="E113" s="23" t="s">
         <v>180</v>
@@ -6735,10 +6739,10 @@
         <v>10097783</v>
       </c>
       <c r="B114" s="23" t="s">
+        <v>607</v>
+      </c>
+      <c r="C114" s="23" t="s">
         <v>608</v>
-      </c>
-      <c r="C114" s="23" t="s">
-        <v>609</v>
       </c>
       <c r="E114" s="23" t="s">
         <v>180</v>
@@ -6752,10 +6756,10 @@
         <v>1088288292</v>
       </c>
       <c r="B115" s="23" t="s">
+        <v>609</v>
+      </c>
+      <c r="C115" s="23" t="s">
         <v>610</v>
-      </c>
-      <c r="C115" s="23" t="s">
-        <v>611</v>
       </c>
       <c r="E115" s="23" t="s">
         <v>180</v>
@@ -6775,10 +6779,10 @@
         <v>1088316247</v>
       </c>
       <c r="B116" s="23" t="s">
+        <v>643</v>
+      </c>
+      <c r="C116" s="23" t="s">
         <v>644</v>
-      </c>
-      <c r="C116" s="23" t="s">
-        <v>645</v>
       </c>
       <c r="E116" s="23" t="s">
         <v>180</v>
@@ -6812,19 +6816,19 @@
         <v>200</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D1" s="23" t="s">
+        <v>412</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>413</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>414</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -9166,28 +9170,28 @@
         <v>181</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" t="s">
         <v>192</v>
       </c>
       <c r="D1" t="s">
+        <v>409</v>
+      </c>
+      <c r="E1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F1" t="s">
         <v>410</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>440</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>411</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>441</v>
-      </c>
-      <c r="H1" t="s">
-        <v>412</v>
-      </c>
-      <c r="I1" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -9603,7 +9607,7 @@
         <v>181</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>207</v>
@@ -9642,112 +9646,112 @@
         <v>218</v>
       </c>
       <c r="O1" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="P1" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="Q1" s="27" t="s">
         <v>375</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="R1" s="27" t="s">
         <v>376</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="S1" s="27" t="s">
         <v>377</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="T1" s="27" t="s">
         <v>378</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="U1" s="27" t="s">
         <v>379</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="V1" s="27" t="s">
         <v>380</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="W1" s="27" t="s">
         <v>381</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="X1" s="27" t="s">
         <v>382</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="Y1" s="27" t="s">
         <v>383</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Z1" s="27" t="s">
         <v>384</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="AA1" s="27" t="s">
         <v>385</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AB1" s="27" t="s">
         <v>386</v>
       </c>
-      <c r="AB1" s="27" t="s">
+      <c r="AC1" s="27" t="s">
         <v>387</v>
       </c>
-      <c r="AC1" s="27" t="s">
+      <c r="AD1" s="27" t="s">
         <v>388</v>
       </c>
-      <c r="AD1" s="27" t="s">
+      <c r="AE1" s="27" t="s">
         <v>389</v>
       </c>
-      <c r="AE1" s="27" t="s">
+      <c r="AF1" s="27" t="s">
         <v>390</v>
       </c>
-      <c r="AF1" s="27" t="s">
+      <c r="AG1" s="27" t="s">
         <v>391</v>
       </c>
-      <c r="AG1" s="27" t="s">
+      <c r="AH1" s="27" t="s">
         <v>392</v>
       </c>
-      <c r="AH1" s="27" t="s">
+      <c r="AI1" s="27" t="s">
         <v>393</v>
       </c>
-      <c r="AI1" s="27" t="s">
+      <c r="AJ1" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="AJ1" s="27" t="s">
+      <c r="AK1" s="27" t="s">
         <v>395</v>
       </c>
-      <c r="AK1" s="27" t="s">
+      <c r="AL1" s="27" t="s">
         <v>396</v>
       </c>
-      <c r="AL1" s="27" t="s">
+      <c r="AM1" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="AM1" s="27" t="s">
+      <c r="AN1" s="27" t="s">
         <v>398</v>
       </c>
-      <c r="AN1" s="27" t="s">
+      <c r="AO1" s="27" t="s">
         <v>399</v>
       </c>
-      <c r="AO1" s="27" t="s">
+      <c r="AP1" s="27" t="s">
         <v>400</v>
       </c>
-      <c r="AP1" s="27" t="s">
+      <c r="AQ1" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="AQ1" s="27" t="s">
+      <c r="AR1" s="27" t="s">
         <v>402</v>
       </c>
-      <c r="AR1" s="27" t="s">
+      <c r="AS1" s="27" t="s">
         <v>403</v>
       </c>
-      <c r="AS1" s="27" t="s">
+      <c r="AT1" s="27" t="s">
         <v>404</v>
       </c>
-      <c r="AT1" s="27" t="s">
+      <c r="AU1" s="27" t="s">
         <v>405</v>
       </c>
-      <c r="AU1" s="27" t="s">
+      <c r="AV1" s="27" t="s">
         <v>406</v>
       </c>
-      <c r="AV1" s="27" t="s">
+      <c r="AW1" s="27" t="s">
         <v>407</v>
       </c>
-      <c r="AW1" s="27" t="s">
+      <c r="AX1" s="27" t="s">
         <v>408</v>
-      </c>
-      <c r="AX1" s="27" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
@@ -11694,7 +11698,7 @@
         <v>181</v>
       </c>
       <c r="B1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" t="s">
         <v>290</v>
@@ -11730,115 +11734,115 @@
         <v>280</v>
       </c>
       <c r="N1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="O1" t="s">
+        <v>449</v>
+      </c>
+      <c r="P1" t="s">
         <v>450</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>451</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>452</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>453</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>454</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>455</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>456</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>457</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>458</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>459</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>460</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>461</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>462</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>463</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>464</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>465</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>466</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>467</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>468</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>469</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>470</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>471</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>472</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>473</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>474</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>475</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>476</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>477</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>478</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>479</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>480</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>481</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>482</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>483</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>484</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
@@ -13943,115 +13947,115 @@
         <v>200</v>
       </c>
       <c r="B1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>338</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>340</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="I1" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="J1" s="26" t="s">
         <v>344</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>345</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="L1" s="26" t="s">
         <v>346</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="M1" s="26" t="s">
         <v>347</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="N1" s="26" t="s">
         <v>348</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="O1" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="P1" s="26" t="s">
         <v>350</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="Q1" s="26" t="s">
         <v>351</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="R1" s="26" t="s">
         <v>352</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="S1" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="T1" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="U1" s="26" t="s">
         <v>355</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="V1" s="26" t="s">
         <v>356</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="W1" s="26" t="s">
         <v>357</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="X1" s="26" t="s">
         <v>358</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="Y1" s="26" t="s">
         <v>359</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="Z1" s="26" t="s">
         <v>360</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="AA1" s="26" t="s">
         <v>361</v>
       </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AB1" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="AB1" s="26" t="s">
+      <c r="AC1" s="26" t="s">
         <v>363</v>
       </c>
-      <c r="AC1" s="26" t="s">
+      <c r="AD1" s="26" t="s">
         <v>364</v>
       </c>
-      <c r="AD1" s="26" t="s">
+      <c r="AE1" s="26" t="s">
         <v>365</v>
       </c>
-      <c r="AE1" s="26" t="s">
+      <c r="AF1" s="26" t="s">
         <v>366</v>
       </c>
-      <c r="AF1" s="26" t="s">
+      <c r="AG1" s="26" t="s">
         <v>367</v>
       </c>
-      <c r="AG1" s="26" t="s">
+      <c r="AH1" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="AH1" s="26" t="s">
+      <c r="AI1" s="26" t="s">
         <v>369</v>
       </c>
-      <c r="AI1" s="26" t="s">
+      <c r="AJ1" s="26" t="s">
         <v>370</v>
       </c>
-      <c r="AJ1" s="26" t="s">
+      <c r="AK1" s="26" t="s">
         <v>371</v>
       </c>
-      <c r="AK1" s="26" t="s">
+      <c r="AL1" s="26" t="s">
         <v>372</v>
-      </c>
-      <c r="AL1" s="26" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
@@ -29971,7 +29975,7 @@
         <v>181</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" s="23" t="s">
         <v>292</v>
@@ -29980,22 +29984,22 @@
         <v>293</v>
       </c>
       <c r="E1" s="23" t="s">
+        <v>433</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>434</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>435</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>436</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>437</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>438</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -30759,9 +30763,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A17E23D-E16A-411D-90B5-242F492A5C36}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -30769,824 +30775,1131 @@
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>200</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>647</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>647</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>182</v>
       </c>
       <c r="B2" s="19">
         <v>45055</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" s="25">
+        <v>45790</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>183</v>
       </c>
       <c r="B3" s="19">
         <v>45027</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" s="25">
+        <v>45755</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>184</v>
       </c>
       <c r="B4" s="19">
         <v>45027</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" s="25">
+        <v>45755</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>185</v>
       </c>
       <c r="B5" s="19">
         <v>45027</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" s="25">
+        <v>45755</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>186</v>
       </c>
       <c r="B6" s="19">
         <v>45027</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D6" s="25">
+        <v>45755</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>187</v>
       </c>
       <c r="B7" s="19">
         <v>45027</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D7" s="25">
+        <v>45755</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="19">
         <v>45028</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D8" s="25">
+        <v>45756</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>189</v>
       </c>
       <c r="B9" s="19">
         <v>45028</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D9" s="25">
+        <v>45756</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>190</v>
       </c>
       <c r="B10" s="19">
         <v>45028</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D10" s="25">
+        <v>45756</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>191</v>
       </c>
       <c r="B11" s="19">
         <v>45028</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11" s="25">
+        <v>45756</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" s="19">
         <v>45028</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D12" s="25">
+        <v>45756</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" s="19">
         <v>45029</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D13" s="25">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" s="19">
         <v>45029</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D14" s="25">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" s="19">
         <v>45029</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D15" s="25">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" s="19">
         <v>45029</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D16" s="25">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" s="19">
         <v>45029</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17" s="25">
+        <v>45757</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" s="19">
         <v>45030</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" s="25">
+        <v>45758</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" s="19">
         <v>45030</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19" s="25">
+        <v>45758</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" s="19">
         <v>45030</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20" s="25">
+        <v>45758</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" s="19">
         <v>45030</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D21" s="25">
+        <v>45758</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" s="19">
         <v>45030</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D22" s="25">
+        <v>45758</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" s="19">
         <v>45033</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D23" s="25">
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" s="19">
         <v>45033</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D24" s="25">
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" s="19">
         <v>45033</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D25" s="25">
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" s="19">
         <v>45033</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D26" s="25">
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" s="19">
         <v>45033</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D27" s="25">
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" s="19">
         <v>45034</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D28" s="25">
+        <v>45769</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" s="19">
         <v>45034</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D29" s="25">
+        <v>45769</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" s="19">
         <v>45034</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D30" s="25">
+        <v>45769</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" s="19">
         <v>45034</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D31" s="25">
+        <v>45769</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" s="19">
         <v>45034</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D32" s="25">
+        <v>45769</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" s="19">
         <v>45035</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D33" s="25">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" s="19">
         <v>45035</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D34" s="25">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
       <c r="B35" s="19">
         <v>45035</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D35" s="25">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" s="19">
         <v>45035</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D36" s="25">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" s="19">
         <v>45035</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D37" s="25">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" s="19">
         <v>45036</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D38" s="25">
+        <v>45771</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39" s="19">
         <v>45036</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D39" s="25">
+        <v>45771</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40" s="19">
         <v>45036</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D40" s="25">
+        <v>45771</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" s="19">
         <v>45036</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D41" s="25">
+        <v>45771</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" s="19">
         <v>45036</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D42" s="25">
+        <v>45771</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43" s="19">
         <v>45037</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D43" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44" s="19">
         <v>45037</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D44" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" s="19">
         <v>45037</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D45" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" s="19">
         <v>45037</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D46" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" s="19">
         <v>45037</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D47" s="25">
+        <v>45772</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" s="19">
         <v>45040</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D48" s="25">
+        <v>45775</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" s="19">
         <v>45040</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D49" s="25">
+        <v>45775</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" s="19">
         <v>45040</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D50" s="25">
+        <v>45775</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" s="19">
         <v>45040</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D51" s="25">
+        <v>45775</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" s="19">
         <v>45040</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D52" s="25">
+        <v>45775</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53" s="19">
         <v>45041</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D53" s="25">
+        <v>45776</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54" s="19">
         <v>45041</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D54" s="25">
+        <v>45776</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55" s="19">
         <v>45041</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D55" s="25">
+        <v>45776</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56" s="19">
         <v>45041</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D56" s="25">
+        <v>45776</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57" s="19">
         <v>45041</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D57" s="25">
+        <v>45776</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58" s="19">
         <v>45042</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D58" s="25">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59" s="19">
         <v>45042</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D59" s="25">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60" s="19">
         <v>45042</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D60" s="25">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61" s="19">
         <v>45042</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D61" s="25">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62" s="19">
         <v>45042</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D62" s="25">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63" s="19">
         <v>45043</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D63" s="25">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64" s="19">
         <v>45043</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D64" s="25">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65" s="19">
         <v>45043</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D65" s="25">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66" s="19">
         <v>45043</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D66" s="25">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67" s="19">
         <v>45043</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D67" s="25">
+        <v>45779</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
       <c r="B68" s="19">
         <v>45044</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D68" s="25">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
       <c r="B69" s="19">
         <v>45044</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D69" s="25">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
       <c r="B70" s="19">
         <v>45044</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D70" s="25">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
       <c r="B71" s="19">
         <v>45044</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D71" s="25">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
       <c r="B72" s="19">
         <v>45044</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D72" s="25">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
       <c r="B73" s="19">
         <v>45048</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D73" s="25">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
       <c r="B74" s="19">
         <v>45048</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D74" s="25">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
       <c r="B75" s="19">
         <v>45048</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D75" s="25">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
       <c r="B76" s="19">
         <v>45048</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D76" s="25">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
       <c r="B77" s="19">
         <v>45048</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D77" s="25">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
       <c r="B78" s="19">
         <v>45049</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D78" s="25">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
       <c r="B79" s="19">
         <v>45049</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D79" s="25">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
       <c r="B80" s="19">
         <v>45049</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D80" s="25">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
       <c r="B81" s="19">
         <v>45049</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D81" s="25">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
       <c r="B82" s="19">
         <v>45049</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D82" s="25">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
       <c r="B83" s="19">
         <v>45050</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D83" s="25">
+        <v>45785</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
       <c r="B84" s="19">
         <v>45050</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D84" s="25">
+        <v>45785</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
       <c r="B85" s="19">
         <v>45050</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D85" s="25">
+        <v>45785</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
       <c r="B86" s="19">
         <v>45050</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D86" s="25">
+        <v>45785</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
       <c r="B87" s="19">
         <v>45050</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D87" s="25">
+        <v>45785</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
       <c r="B88" s="19">
         <v>45051</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D88" s="25">
+        <v>45786</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
       <c r="B89" s="19">
         <v>45051</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D89" s="25">
+        <v>45786</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90" s="19">
         <v>45051</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D90" s="25">
+        <v>45786</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
       <c r="B91" s="19">
         <v>45051</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D91" s="25">
+        <v>45786</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
       <c r="B92" s="19">
         <v>45051</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D92" s="25">
+        <v>45786</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
       <c r="B93" s="19">
         <v>45054</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D93" s="25">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
       <c r="B94" s="19">
         <v>45054</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D94" s="25">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
       <c r="B95" s="19">
         <v>45054</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D95" s="25">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
       <c r="B96" s="19">
         <v>45054</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D96" s="25">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
       <c r="B97" s="19">
         <v>45054</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D97" s="25">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
       <c r="B98" s="19">
         <v>45055</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D98" s="25">
+        <v>45790</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
       <c r="B99" s="19">
         <v>45055</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D99" s="25">
+        <v>45790</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
       <c r="B100" s="19">
         <v>45055</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D100" s="25">
+        <v>45790</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
       <c r="B101" s="19">
         <v>45055</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D101" s="25">
+        <v>45790</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B106" s="19"/>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B107" s="19"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B108" s="19"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -31614,19 +31927,19 @@
         <v>181</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E1" s="23" t="s">
+        <v>444</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>445</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>446</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -33220,19 +33533,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E1" t="s">
         <v>318</v>
       </c>
-      <c r="B1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E1" t="s">
-        <v>319</v>
-      </c>
       <c r="F1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -33241,7 +33554,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C65" si="1">IF(OR(WEEKDAY(E2,1)=1,WEEKDAY(E2,1)=7,B2="F"),"n","h")</f>
@@ -33369,7 +33682,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
@@ -34765,7 +35078,7 @@
         <v>2</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="7"/>
@@ -34821,7 +35134,7 @@
         <v>5</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="7"/>
@@ -34841,7 +35154,7 @@
         <v>6</v>
       </c>
       <c r="B90" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="7"/>
@@ -35445,7 +35758,7 @@
         <v>4</v>
       </c>
       <c r="B123" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C123" t="str">
         <f t="shared" si="7"/>
@@ -35663,7 +35976,7 @@
         <v>2</v>
       </c>
       <c r="B135" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C135" t="str">
         <f t="shared" si="12"/>
@@ -36047,7 +36360,7 @@
         <v>2</v>
       </c>
       <c r="B156" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C156" t="str">
         <f t="shared" si="12"/>
@@ -36175,7 +36488,7 @@
         <v>2</v>
       </c>
       <c r="B163" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C163" t="str">
         <f t="shared" si="12"/>
@@ -36559,7 +36872,7 @@
         <v>2</v>
       </c>
       <c r="B184" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C184" t="str">
         <f t="shared" si="12"/>
@@ -37231,7 +37544,7 @@
         <v>4</v>
       </c>
       <c r="B221" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C221" t="str">
         <f t="shared" si="16"/>
@@ -37449,7 +37762,7 @@
         <v>2</v>
       </c>
       <c r="B233" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C233" t="str">
         <f t="shared" si="16"/>
@@ -38467,7 +38780,7 @@
         <v>2</v>
       </c>
       <c r="B289" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C289" t="str">
         <f t="shared" si="20"/>
@@ -38851,7 +39164,7 @@
         <v>2</v>
       </c>
       <c r="B310" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C310" t="str">
         <f t="shared" si="20"/>
@@ -38979,7 +39292,7 @@
         <v>2</v>
       </c>
       <c r="B317" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C317" t="str">
         <f t="shared" si="20"/>
@@ -39777,7 +40090,7 @@
         <v>4</v>
       </c>
       <c r="B361" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C361" t="str">
         <f t="shared" si="24"/>
@@ -39909,7 +40222,7 @@
         <v>4</v>
       </c>
       <c r="B368" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C368" t="str">
         <f t="shared" si="24"/>
@@ -40001,7 +40314,7 @@
         <v>2</v>
       </c>
       <c r="B373" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C373" t="str">
         <f t="shared" si="24"/>
@@ -41397,7 +41710,7 @@
         <v>2</v>
       </c>
       <c r="B450" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C450" t="str">
         <f t="shared" ref="C450:C513" si="32">IF(OR(WEEKDAY(E450,1)=1,WEEKDAY(E450,1)=7,B450="F"),"n","h")</f>
@@ -41835,7 +42148,7 @@
         <v>5</v>
       </c>
       <c r="B474" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C474" t="str">
         <f t="shared" si="32"/>
@@ -41855,7 +42168,7 @@
         <v>6</v>
       </c>
       <c r="B475" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C475" t="str">
         <f t="shared" si="32"/>
@@ -42095,7 +42408,7 @@
         <v>5</v>
       </c>
       <c r="B488" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C488" t="str">
         <f t="shared" si="32"/>
@@ -42677,7 +42990,7 @@
         <v>2</v>
       </c>
       <c r="B520" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C520" t="str">
         <f t="shared" si="36"/>
@@ -43057,7 +43370,7 @@
         <v>2</v>
       </c>
       <c r="B541" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C541" t="str">
         <f t="shared" si="36"/>
@@ -43185,7 +43498,7 @@
         <v>2</v>
       </c>
       <c r="B548" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C548" t="str">
         <f t="shared" si="36"/>
@@ -43879,7 +44192,7 @@
         <v>5</v>
       </c>
       <c r="B586" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C586" t="str">
         <f t="shared" si="41"/>
@@ -44079,7 +44392,7 @@
         <v>2</v>
       </c>
       <c r="B597" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C597" t="str">
         <f t="shared" si="41"/>
@@ -45097,7 +45410,7 @@
         <v>2</v>
       </c>
       <c r="B653" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C653" t="str">
         <f t="shared" si="45"/>
@@ -45481,7 +45794,7 @@
         <v>2</v>
       </c>
       <c r="B674" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C674" t="str">
         <f t="shared" si="45"/>
@@ -45735,7 +46048,7 @@
         <v>2</v>
       </c>
       <c r="B688" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C688" t="str">
         <f t="shared" si="45"/>
@@ -46119,7 +46432,7 @@
         <v>2</v>
       </c>
       <c r="B709" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C709" t="str">
         <f t="shared" si="49"/>
@@ -46427,7 +46740,7 @@
         <v>5</v>
       </c>
       <c r="B726" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C726" t="str">
         <f t="shared" si="49"/>
@@ -46559,7 +46872,7 @@
         <v>5</v>
       </c>
       <c r="B733" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C733" t="str">
         <f t="shared" si="49"/>
@@ -46759,7 +47072,7 @@
         <v>2</v>
       </c>
       <c r="B744" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C744" t="str">
         <f t="shared" si="49"/>
@@ -48029,7 +48342,7 @@
         <v>2</v>
       </c>
       <c r="B814" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C814" t="str">
         <f t="shared" si="53"/>
@@ -48215,7 +48528,7 @@
         <v>5</v>
       </c>
       <c r="B824" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C824" t="str">
         <f t="shared" si="53"/>
@@ -48235,7 +48548,7 @@
         <v>6</v>
       </c>
       <c r="B825" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C825" t="str">
         <f t="shared" si="53"/>
@@ -48745,7 +49058,7 @@
         <v>6</v>
       </c>
       <c r="B853" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C853" t="str">
         <f t="shared" si="57"/>
@@ -49053,7 +49366,7 @@
         <v>2</v>
       </c>
       <c r="B870" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C870" t="str">
         <f t="shared" si="57"/>
@@ -49437,7 +49750,7 @@
         <v>2</v>
       </c>
       <c r="B891" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C891" t="str">
         <f t="shared" si="57"/>
@@ -49565,7 +49878,7 @@
         <v>2</v>
       </c>
       <c r="B898" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C898" t="str">
         <f t="shared" ref="C898:C961" si="61">IF(OR(WEEKDAY(E898,1)=1,WEEKDAY(E898,1)=7,B898="F"),"n","h")</f>
@@ -49819,7 +50132,7 @@
         <v>2</v>
       </c>
       <c r="B912" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C912" t="str">
         <f t="shared" si="61"/>
@@ -50203,7 +50516,7 @@
         <v>2</v>
       </c>
       <c r="B933" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C933" t="str">
         <f t="shared" si="61"/>
@@ -50533,7 +50846,7 @@
         <v>6</v>
       </c>
       <c r="B951" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C951" t="str">
         <f t="shared" si="61"/>
@@ -50715,7 +51028,7 @@
         <v>2</v>
       </c>
       <c r="B961" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C961" t="str">
         <f t="shared" si="61"/>
@@ -51733,7 +52046,7 @@
         <v>2</v>
       </c>
       <c r="B1017" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C1017" t="str">
         <f t="shared" si="65"/>
@@ -52117,7 +52430,7 @@
         <v>2</v>
       </c>
       <c r="B1038" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C1038" t="str">
         <f t="shared" si="69"/>
@@ -52371,7 +52684,7 @@
         <v>2</v>
       </c>
       <c r="B1052" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C1052" t="str">
         <f t="shared" si="69"/>
@@ -52773,7 +53086,7 @@
         <v>3</v>
       </c>
       <c r="B1074" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C1074" t="str">
         <f t="shared" si="69"/>
@@ -53081,7 +53394,7 @@
         <v>6</v>
       </c>
       <c r="B1091" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C1091" t="str">
         <f t="shared" si="73"/>
@@ -53195,7 +53508,7 @@
         <v>6</v>
       </c>
       <c r="B1097" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C1097" t="str">
         <f t="shared" si="73"/>
@@ -53368,7 +53681,7 @@
         <v>2</v>
       </c>
       <c r="B1107" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C1107" t="str">
         <f t="shared" si="73"/>
@@ -53753,7 +54066,7 @@
         <v>262</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -53916,22 +54229,22 @@
         <v>268</v>
       </c>
       <c r="H1" t="s">
+        <v>549</v>
+      </c>
+      <c r="I1" t="s">
         <v>550</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>551</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>552</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>553</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>554</v>
-      </c>
-      <c r="M1" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -54354,7 +54667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22978039-1543-4DF0-A3D8-F1CAD6292EF2}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -54372,7 +54685,7 @@
         <v>181</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -54513,46 +54826,46 @@
         <v>261</v>
       </c>
       <c r="J1" s="25" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="K1" s="25" t="s">
+        <v>555</v>
+      </c>
+      <c r="L1" s="25" t="s">
         <v>556</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="M1" s="25" t="s">
         <v>557</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="N1" s="25" t="s">
         <v>558</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="O1" s="25" t="s">
         <v>559</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="P1" s="25" t="s">
         <v>560</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="Q1" s="25" t="s">
         <v>561</v>
       </c>
-      <c r="Q1" s="25" t="s">
-        <v>562</v>
-      </c>
       <c r="R1" s="25" t="s">
+        <v>619</v>
+      </c>
+      <c r="S1" s="25" t="s">
         <v>620</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="T1" s="25" t="s">
         <v>621</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="U1" s="25" t="s">
         <v>622</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="V1" s="25" t="s">
         <v>623</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="W1" s="25" t="s">
         <v>624</v>
-      </c>
-      <c r="W1" s="25" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -55293,7 +55606,7 @@
         <v>181</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -55419,40 +55732,40 @@
         <v>253</v>
       </c>
       <c r="H1" t="s">
+        <v>562</v>
+      </c>
+      <c r="I1" t="s">
         <v>563</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>564</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>565</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>566</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>567</v>
       </c>
-      <c r="M1" t="s">
-        <v>568</v>
-      </c>
       <c r="N1" t="s">
+        <v>625</v>
+      </c>
+      <c r="O1" t="s">
         <v>626</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>627</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>628</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>629</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>630</v>
-      </c>
-      <c r="S1" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -56092,22 +56405,22 @@
         <v>234</v>
       </c>
       <c r="H1" t="s">
+        <v>541</v>
+      </c>
+      <c r="I1" t="s">
         <v>542</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>543</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>544</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>545</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>546</v>
-      </c>
-      <c r="M1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -56555,13 +56868,13 @@
         <v>226</v>
       </c>
       <c r="E1" s="25" t="s">
+        <v>538</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>539</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>540</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -56822,10 +57135,10 @@
         <v>225</v>
       </c>
       <c r="C1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -57011,40 +57324,40 @@
         <v>240</v>
       </c>
       <c r="H1" t="s">
+        <v>579</v>
+      </c>
+      <c r="I1" t="s">
         <v>580</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>581</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>582</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>583</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>584</v>
       </c>
-      <c r="M1" t="s">
-        <v>585</v>
-      </c>
       <c r="N1" t="s">
+        <v>632</v>
+      </c>
+      <c r="O1" t="s">
         <v>633</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>634</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>635</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>636</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>637</v>
-      </c>
-      <c r="S1" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -57682,7 +57995,7 @@
         <v>181</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>193</v>
@@ -57700,61 +58013,61 @@
         <v>197</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I1" s="20" t="s">
+        <v>512</v>
+      </c>
+      <c r="J1" s="20" t="s">
         <v>513</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="K1" s="20" t="s">
         <v>514</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="L1" s="20" t="s">
         <v>515</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="M1" s="20" t="s">
         <v>516</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="N1" s="20" t="s">
         <v>517</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="O1" s="20" t="s">
         <v>518</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="P1" s="20" t="s">
         <v>519</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="Q1" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="R1" s="20" t="s">
         <v>521</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="20" t="s">
         <v>522</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="T1" s="20" t="s">
         <v>523</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="U1" s="20" t="s">
         <v>524</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="V1" s="20" t="s">
         <v>525</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="W1" s="20" t="s">
         <v>526</v>
       </c>
-      <c r="W1" s="20" t="s">
+      <c r="X1" s="20" t="s">
         <v>527</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="Y1" s="20" t="s">
         <v>528</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="Z1" s="20" t="s">
         <v>529</v>
-      </c>
-      <c r="Z1" s="20" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -58775,10 +59088,10 @@
         <v>241</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E1" s="25"/>
     </row>
@@ -58966,40 +59279,40 @@
         <v>247</v>
       </c>
       <c r="H1" t="s">
+        <v>570</v>
+      </c>
+      <c r="I1" t="s">
         <v>571</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>572</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>573</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>574</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>575</v>
       </c>
-      <c r="M1" t="s">
-        <v>576</v>
-      </c>
       <c r="N1" t="s">
+        <v>612</v>
+      </c>
+      <c r="O1" t="s">
         <v>613</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>614</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>615</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>616</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>617</v>
-      </c>
-      <c r="S1" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -59641,10 +59954,10 @@
         <v>219</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>447</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>448</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -59954,10 +60267,10 @@
         <v>222</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -60129,10 +60442,10 @@
         <v>224</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -60303,7 +60616,7 @@
         <v>223</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -60441,16 +60754,16 @@
         <v>200</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>532</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>533</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -62202,19 +62515,19 @@
         <v>181</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>295</v>
@@ -62232,61 +62545,61 @@
         <v>299</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="M1" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="N1" s="20" t="s">
         <v>416</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="O1" s="20" t="s">
         <v>417</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="P1" s="20" t="s">
         <v>418</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="Q1" s="20" t="s">
         <v>419</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="R1" s="20" t="s">
         <v>420</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="20" t="s">
         <v>421</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="T1" s="20" t="s">
         <v>422</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="U1" s="20" t="s">
         <v>423</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="V1" s="20" t="s">
         <v>424</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="W1" s="20" t="s">
         <v>425</v>
       </c>
-      <c r="W1" s="20" t="s">
+      <c r="X1" s="20" t="s">
         <v>426</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="Y1" s="20" t="s">
         <v>427</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="Z1" s="20" t="s">
         <v>428</v>
       </c>
-      <c r="Z1" s="20" t="s">
+      <c r="AA1" s="20" t="s">
         <v>429</v>
       </c>
-      <c r="AA1" s="20" t="s">
+      <c r="AB1" s="20" t="s">
         <v>430</v>
       </c>
-      <c r="AB1" s="20" t="s">
+      <c r="AC1" s="20" t="s">
         <v>431</v>
       </c>
-      <c r="AC1" s="20" t="s">
+      <c r="AD1" s="20" t="s">
         <v>432</v>
-      </c>
-      <c r="AD1" s="20" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -63433,7 +63746,7 @@
         <v>181</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>300</v>
@@ -63451,61 +63764,61 @@
         <v>304</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I1" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="J1" s="20" t="s">
         <v>486</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="K1" s="20" t="s">
         <v>487</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="L1" s="20" t="s">
         <v>488</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="M1" s="20" t="s">
         <v>489</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="N1" s="20" t="s">
         <v>490</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="O1" s="20" t="s">
         <v>491</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="P1" s="20" t="s">
         <v>492</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="Q1" s="20" t="s">
         <v>493</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="R1" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="20" t="s">
         <v>495</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="T1" s="20" t="s">
         <v>496</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="U1" s="20" t="s">
         <v>497</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="V1" s="20" t="s">
         <v>498</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="W1" s="20" t="s">
         <v>499</v>
       </c>
-      <c r="W1" s="20" t="s">
+      <c r="X1" s="20" t="s">
         <v>500</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="Y1" s="20" t="s">
         <v>501</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="Z1" s="20" t="s">
         <v>502</v>
-      </c>
-      <c r="Z1" s="20" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -64523,7 +64836,7 @@
         <v>181</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" t="s">
         <v>198</v>
@@ -64532,34 +64845,34 @@
         <v>199</v>
       </c>
       <c r="E1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F1" t="s">
+        <v>503</v>
+      </c>
+      <c r="G1" t="s">
         <v>504</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>505</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>506</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>507</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>508</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>509</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>510</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>511</v>
-      </c>
-      <c r="N1" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -65135,7 +65448,7 @@
         <v>181</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" s="23" t="s">
         <v>204</v>
@@ -65147,31 +65460,31 @@
         <v>206</v>
       </c>
       <c r="F1" s="23" t="s">
+        <v>321</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>322</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>323</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>324</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>325</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>326</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>327</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="M1" s="23" t="s">
         <v>328</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="N1" s="23" t="s">
         <v>329</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -65737,7 +66050,7 @@
         <v>181</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>202</v>
@@ -65746,22 +66059,22 @@
         <v>203</v>
       </c>
       <c r="F1" s="23" t="s">
+        <v>331</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>333</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>334</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>336</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -67822,19 +68135,19 @@
         <v>200</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C1" s="23" t="s">
         <v>201</v>
       </c>
       <c r="D1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>